<commit_message>
[FE - Edit] Download Template Budget Planning
</commit_message>
<xml_diff>
--- a/budgetin/api/utils/template/import_template_budget.xlsx
+++ b/budgetin/api/utils/template/import_template_budget.xlsx
@@ -1505,7 +1505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1533,12 +1533,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BI006</t>
+          <t>BA001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Data Center - Infrastructure</t>
+          <t>Acquiring</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1550,29 +1550,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BG001</t>
+          <t>BA002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Governance - Process</t>
+          <t>API</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BG002</t>
+          <t>BA003</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Governance - IT Management Office</t>
+          <t>ATM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1584,59 +1584,63 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BA001</t>
+          <t>BA007</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Acquiring</t>
+          <t>BDS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BA003</t>
+          <t>BA009</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>BO Support</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BA007</t>
+          <t>BA010</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BDS</t>
+          <t>Cash Operation</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BA022</t>
+          <t>BA011</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Future Branch </t>
+          <t>Corporate Banking</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1648,29 +1652,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BA058</t>
+          <t>BA012</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Low Code Digital Factory</t>
+          <t>H2H (Host to Host)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BA069</t>
+          <t>BA013</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Digital Innovation Solution - Process</t>
+          <t>KBB (KlikBCA Bisnis)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1682,59 +1686,63 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BA072</t>
+          <t>BA016</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Application Management - Technology</t>
+          <t>Credit Card</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BC001</t>
+          <t>BA018</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Compliance - Process</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+          <t>Credit SME</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BC002</t>
+          <t>BA020</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Compliance - Technology</t>
+          <t xml:space="preserve">Customer Relationship Value </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BD001</t>
+          <t>BA021</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Data Management - Data Analytics</t>
+          <t>Digital Branch</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1746,29 +1754,29 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BD002</t>
+          <t>BA022</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Data Management - Masterdata</t>
+          <t xml:space="preserve">Future Branch </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BD003</t>
+          <t>BA023</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data Management - Data Integration </t>
+          <t>Halo BCA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1780,29 +1788,29 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BD004</t>
+          <t>BA024</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Data Management - Data Streaming</t>
+          <t>Application Development-Human Capital Application</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BD005</t>
+          <t>BA025</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Data Management - Data Collection</t>
+          <t>Application Development-Learning &amp; Development Application</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1814,25 +1822,29 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BI001</t>
+          <t>BA026</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Mainframe</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
+          <t>International Trade</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BI003</t>
+          <t>BA029</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - EAI</t>
+          <t>KBI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1844,29 +1856,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BI004</t>
+          <t>BA030</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Open System</t>
+          <t>Kliring</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BI005</t>
+          <t>BA032</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Data Center - Operation</t>
+          <t>Branchless Banking</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1878,29 +1890,29 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BI009</t>
+          <t>BA034</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Network - Data Center</t>
+          <t>Sakuku</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BI010</t>
+          <t>BA035</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Network - Voice</t>
+          <t>m-BCA</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1912,59 +1924,63 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BS003</t>
+          <t>BA036</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Security System</t>
+          <t>VIRA (ChatBanking)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BI007</t>
+          <t xml:space="preserve">BA038 </t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Data Center - Facility</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
+          <t xml:space="preserve"> myBCA Portal</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BA002</t>
+          <t>BA043</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>API</t>
+          <t>e-Statement</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BA009</t>
+          <t>BA047</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BO Support</t>
+          <t>Relationship Platform</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1976,29 +1992,29 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BA010</t>
+          <t>BA048</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cash Operation</t>
+          <t>Remittance</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BA011</t>
+          <t>BA049</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Corporate Banking</t>
+          <t>Sub Account</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2010,29 +2026,29 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BA013</t>
+          <t>BA050</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>KBB (KlikBCA Bisnis)</t>
+          <t>Treasury</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BA020</t>
+          <t>BA058</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Customer Relationship Value </t>
+          <t>Low Code Digital Factory</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2044,25 +2060,29 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BA021</t>
+          <t>BA059</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Digital Branch</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
+          <t>Omni Channel</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BA023</t>
+          <t>BA062</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Halo BCA</t>
+          <t>Application Development-Pendukung Logistik</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2074,29 +2094,29 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BA024</t>
+          <t>BA063</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Application Development-Human Capital Application</t>
+          <t>Pendukung Layanan Perbankan Eletronik</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BA025</t>
+          <t>BA066</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Application Development-Learning &amp; Development Application</t>
+          <t>Pendukung Audit Internal</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2108,29 +2128,29 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>BA029</t>
+          <t>BA067</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>KBI</t>
+          <t>Pendukung Finance &amp; Accounting</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BA030</t>
+          <t>BA069</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Kliring</t>
+          <t>Digital Innovation Solution - Process</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2142,59 +2162,63 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BA035</t>
+          <t>BA070</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>m-BCA</t>
+          <t>Digital Innovation Solution - Technology</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BA036</t>
+          <t>BA071</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VIRA (ChatBanking)</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr"/>
+          <t>Application Management - Process</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>BA038</t>
+          <t>BA072</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>- myBCA Portal</t>
+          <t>Application Management - Technology</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BA048</t>
+          <t>BA073</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Remittance</t>
+          <t>Chat Service</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2206,29 +2230,29 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BA049</t>
+          <t>BC001</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Sub Account</t>
+          <t>Compliance - Process</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>BA050</t>
+          <t>BC002</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Treasury</t>
+          <t>Compliance - Technology</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2240,29 +2264,29 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>BA059</t>
+          <t>BC007</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Omni Channel</t>
+          <t>Compliance Technology - APU - PPT</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>BA062</t>
+          <t>BC008</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Application Development-Pendukung Logistik</t>
+          <t>Compliance Technology - Support Kebijakan Akuntansi</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2274,25 +2298,29 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>BA063</t>
+          <t>BC010</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Pendukung Layanan Perbankan Eletronik</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
+          <t>Compliance Technology - Laporan Keuangan Regulator</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>BA067</t>
+          <t>BC071</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Pendukung Finance &amp; Accounting</t>
+          <t>Application Development-Process</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2304,29 +2332,29 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BA070</t>
+          <t>BD001</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Digital Innovation Solution - Technology</t>
+          <t>Data Management - Data Analytics</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BA071</t>
+          <t>BD002</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Application Management - Process</t>
+          <t>Data Management - Masterdata</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2338,29 +2366,29 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>BC007</t>
+          <t>BD003</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Compliance Technology - APU - PPT</t>
+          <t xml:space="preserve">Data Management - Data Integration </t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BC008</t>
+          <t>BD004</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Compliance Technology - Support Kebijakan Akuntansi</t>
+          <t>Data Management - Data Streaming</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2372,29 +2400,29 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BI008</t>
+          <t>BD005</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Network - Cabang</t>
+          <t>Data Management - Data Collection</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>BI013</t>
+          <t>BG001</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>PC &amp; Laptop</t>
+          <t>Governance - Process</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2406,46 +2434,46 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BR002</t>
+          <t>BG002</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Risk - Technology</t>
+          <t>Governance - IT Management Office</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Run the Business</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BR003</t>
+          <t>BI001</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Risk Technology - IRMIS </t>
+          <t>Infrastruktur IT - Mainframe</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BR004</t>
+          <t>BI002</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Risk Technology - ORMIS</t>
+          <t>Infrastruktur IT - Tandem</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2457,59 +2485,63 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BS001</t>
+          <t>BI003</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Security Management - Process</t>
+          <t>Infrastruktur IT - EAI</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BA012</t>
+          <t>BI004</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>H2H (Host to Host)</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr"/>
+          <t>Infrastruktur IT - Open System</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Run the Business</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BA016</t>
+          <t>BI005</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Credit Card</t>
+          <t>Infrastruktur IT - Data Center - Operation</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BA018</t>
+          <t>BI006</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Credit SME</t>
+          <t>Infrastruktur IT - Data Center - Infrastructure</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2521,29 +2553,29 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BA026</t>
+          <t>BI007</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>International Trade</t>
+          <t>Infrastruktur IT - Data Center - Facility</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BA032</t>
+          <t>BI008</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Branchless Banking</t>
+          <t>Infrastruktur IT - Network - Cabang</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2555,29 +2587,29 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BA034</t>
+          <t>BI009</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Sakuku</t>
+          <t>Infrastruktur IT - Network - Data Center</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>BA043</t>
+          <t>BI010</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>e-Statement</t>
+          <t>Infrastruktur IT - Network - Voice</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2589,25 +2621,29 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>BA047</t>
+          <t>BI013</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Relationship Platform</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr"/>
+          <t>PC &amp; Laptop</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Run the Business</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BC071</t>
+          <t>BR002</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Application Development-Process</t>
+          <t>Risk - Technology</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2619,29 +2655,29 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BI002</t>
+          <t>BR003</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Infrastruktur IT - Tandem</t>
+          <t xml:space="preserve">Risk Technology - IRMIS </t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>BA066</t>
+          <t>BR004</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Pendukung Audit Internal</t>
+          <t>Risk Technology - ORMIS</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2653,29 +2689,29 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BA073</t>
+          <t>BS001</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Chat Service</t>
+          <t>Security Management - Process</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BC010</t>
+          <t>BS003</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Compliance Technology - Laporan Keuangan Regulator</t>
+          <t>Security System</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2697,24 +2733,58 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>BA1012</t>
+          <t>BT001</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>Test Product 01</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Grow the Business</t>
+          <t>Run the Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>BT002</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Test Product 02</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>BT003</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Test Product 03</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2757,255 +2827,357 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ASET ROA TANAH</t>
+          <t>Keperluan Komputer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hyperion ASET ROA TANAH</t>
+          <t>Keperluan Komputer</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>COA untuk ASET ROA TANAH</t>
+          <t>COA untuk Keperluan Komputer</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Biaya Pengelola Pendukung Operasional</t>
+          <t>M. HW</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hyperion Biaya Pengelola Pendukung Operasional</t>
+          <t>Maintenance Hardware</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>COA untuk Biaya Pengelola Pendukung Operasional</t>
+          <t>COA untuk Maintenance Hardware</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Biaya Pengelola Pendukung Proses</t>
+          <t>Test COA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hyperion Biaya Pengelola Pendukung Proses</t>
+          <t>Hype COA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>COA untuk Biaya Pengelola Pendukung Proses</t>
+          <t>Def COA</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Consultant</t>
+          <t>Coa 1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hyperion Consultant</t>
+          <t>Coa 3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>COA untuk Consultant</t>
+          <t>Coa 2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Gedung</t>
+          <t>Coa 2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hyperion Gedung</t>
+          <t>Coa 2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>COA untuk Gedung</t>
+          <t>Coa 2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HW</t>
+          <t>Coa 3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hyperion HW</t>
+          <t>Coa 3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>COA untuk HW</t>
+          <t>Coa 3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Keperluan Kantor Lainnya</t>
+          <t>Coa 4</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Hyperion Keperluan Kantor Lainnya</t>
+          <t>Coa 4</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>COA untuk Keperluan Kantor Lainnya</t>
+          <t>Coa 4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Keperluan Komputer</t>
+          <t>Coa 5</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hyperion Keperluan Komputer</t>
+          <t>Coa 5</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>COA untuk Keperluan Komputer</t>
+          <t>Coa 5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>M. HW</t>
+          <t>Gedung</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hyperion M. HW</t>
+          <t>Gedung Hyperion</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>COA untuk M. HW</t>
+          <t>COA untuk Gedung</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>M. SW</t>
+          <t>ASET ROA TANAH</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hyperion M. SW</t>
+          <t>ROA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>COA untuk M. SW</t>
+          <t>COA untuk Roa Tanah</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Pemanfaatan IT</t>
+          <t>Pemeliharaan Gedung &amp; Perabotan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hyperion Pemanfaatan IT</t>
+          <t>M.Gedung&amp;Perabotan</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>COA untuk Pemanfaatan IT</t>
+          <t>COA untuk Maintenance Gedung &amp; Perabotan</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Pemeliharaan Gedung &amp; Perabotan</t>
+          <t>SW</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hyperion Pemeliharaan Gedung &amp; Perabotan</t>
+          <t>Software</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>COA untuk Pemeliharaan Gedung &amp; Perabotan</t>
+          <t>COA untuk Software</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Promosi</t>
+          <t>HW</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Hyperion Promosi</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>COA untuk Promosi</t>
+          <t>COA untuk Hardware</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sewa Gedung</t>
+          <t>M. SW</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hyperion Sewa Gedung</t>
+          <t>Maintenance Software</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>COA untuk Sewa Gedung</t>
+          <t>COA untuk Maintenance Software</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>Consultant</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hyperion SW</t>
+          <t>Consultant</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>COA untuk SW</t>
+          <t>COA untuk Consultant</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Pemanfaatan IT</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Pemanfaatan IT</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>COA untuk pemanfaatan IT</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sewa Gedung</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Sewa Gedung</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>COA untuk Sewa Gedung</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Keperluan Kantor Lainnya</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>COA untuk keperluan kantor lainnya</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Biaya Pengelola Pendukung Operasional</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Biaya Pengelola Pendukung Operator</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>COA Pendukung Operator</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Promosi</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Promosi</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>COA untuk Promosi</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Biaya Pengelola Pendukung Proses</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Pengelola Pendukung Proses</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>COA untuk Biaya Pengelola Pendukung Proses</t>
         </is>
       </c>
     </row>

</xml_diff>